<commit_message>
Updated SGU template file and added more species to code list.
</commit_message>
<xml_diff>
--- a/inst/extdata/codelist_wtse.xlsx
+++ b/inst/extdata/codelist_wtse.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\projects\data\contaminants\MoCiS2.wtse\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82863E-BE6D-4EE7-A2AE-AF35F301C7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATIONER" sheetId="14" r:id="rId1"/>
@@ -20,25 +21,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PARAMETRAR!$A$1:$Q$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STATIONER!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="939">
   <si>
     <t>PERC</t>
   </si>
@@ -2831,12 +2819,36 @@
   </si>
   <si>
     <t>CH12/283</t>
+  </si>
+  <si>
+    <t>BLAG</t>
+  </si>
+  <si>
+    <t>Fjallvrak</t>
+  </si>
+  <si>
+    <t>Buteo lagopus</t>
+  </si>
+  <si>
+    <t>FPER</t>
+  </si>
+  <si>
+    <t>Pilgrimsfalk</t>
+  </si>
+  <si>
+    <t>Falco peregrinus</t>
+  </si>
+  <si>
+    <t>Fiskgjuse</t>
+  </si>
+  <si>
+    <t>Pandion haliaeetus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2934,7 +2946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3008,8 +3020,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4200,7 +4210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:D331"/>
   <sheetViews>
@@ -8852,20 +8862,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Blad2"/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8890,268 +8900,268 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="C2">
-        <v>206198</v>
+        <v>100011</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>934</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>935</v>
       </c>
       <c r="C3">
-        <v>106665</v>
+        <v>100054</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>936</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>242</v>
       </c>
       <c r="C4">
-        <v>102618</v>
+        <v>100067</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>206139</v>
+        <v>232</v>
+      </c>
+      <c r="C5" s="4">
+        <v>100068</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>937</v>
       </c>
       <c r="C6">
-        <v>206231</v>
+        <v>100096</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>938</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>248</v>
       </c>
       <c r="C7">
-        <v>100144</v>
+        <v>100102</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>233</v>
       </c>
       <c r="C8">
-        <v>102950</v>
+        <v>100104</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>206293</v>
+        <v>100144</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>931</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>932</v>
       </c>
       <c r="C10">
-        <v>206142</v>
+        <v>102110</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>933</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>206089</v>
+        <v>102618</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C12">
-        <v>206135</v>
+        <v>102708</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>102708</v>
+        <v>102950</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
-      </c>
-      <c r="C14" s="4">
-        <v>100068</v>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>106665</v>
       </c>
       <c r="D14" t="s">
-        <v>235</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>233</v>
+        <v>123</v>
       </c>
       <c r="C15">
-        <v>100104</v>
+        <v>206089</v>
       </c>
       <c r="D15" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="B16" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="C16">
-        <v>100067</v>
+        <v>206135</v>
       </c>
       <c r="D16" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>100011</v>
+        <v>206139</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>248</v>
+        <v>15</v>
       </c>
       <c r="C18">
-        <v>100102</v>
+        <v>206142</v>
       </c>
       <c r="D18" t="s">
-        <v>249</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B19" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C19">
-        <v>262067</v>
+        <v>206197</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>206197</v>
+        <v>206198</v>
       </c>
       <c r="D20" t="s">
-        <v>255</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -9168,20 +9178,65 @@
         <v>258</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>206231</v>
+      </c>
+      <c r="D22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23">
+        <v>206293</v>
+      </c>
+      <c r="D23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" t="s">
+        <v>251</v>
+      </c>
+      <c r="C24">
+        <v>262067</v>
+      </c>
+      <c r="D24" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
+    <sortCondition ref="C2:C24"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Blad3">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13271,7 +13326,7 @@
       <c r="B106" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="C106" s="38" t="s">
+      <c r="C106" s="21" t="s">
         <v>930</v>
       </c>
       <c r="D106" t="s">
@@ -13307,7 +13362,7 @@
       <c r="B107" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="C107" s="37" t="s">
+      <c r="C107" s="20" t="s">
         <v>929</v>
       </c>
       <c r="D107" s="20" t="s">
@@ -13345,7 +13400,7 @@
       <c r="A108" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B108" s="40"/>
+      <c r="B108" s="38"/>
       <c r="C108" s="24"/>
       <c r="D108" t="s">
         <v>297</v>
@@ -13379,7 +13434,7 @@
       <c r="A109" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="B109" s="40"/>
+      <c r="B109" s="38"/>
       <c r="C109" s="24"/>
       <c r="D109" t="s">
         <v>297</v>
@@ -13413,7 +13468,7 @@
       <c r="A110" s="24" t="s">
         <v>283</v>
       </c>
-      <c r="B110" s="40"/>
+      <c r="B110" s="38"/>
       <c r="C110" s="24"/>
       <c r="D110" t="s">
         <v>297</v>
@@ -13447,7 +13502,7 @@
       <c r="A111" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="B111" s="40"/>
+      <c r="B111" s="38"/>
       <c r="C111" s="24"/>
       <c r="D111" t="s">
         <v>297</v>
@@ -13481,7 +13536,7 @@
       <c r="A112" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="B112" s="40"/>
+      <c r="B112" s="38"/>
       <c r="C112" s="24"/>
       <c r="D112" t="s">
         <v>297</v>
@@ -13515,7 +13570,7 @@
       <c r="A113" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="B113" s="40"/>
+      <c r="B113" s="38"/>
       <c r="C113" s="24"/>
       <c r="D113" t="s">
         <v>297</v>
@@ -13549,7 +13604,7 @@
       <c r="A114" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="B114" s="40"/>
+      <c r="B114" s="38"/>
       <c r="C114" s="24"/>
       <c r="D114" t="s">
         <v>297</v>
@@ -13583,7 +13638,7 @@
       <c r="A115" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="B115" s="40"/>
+      <c r="B115" s="38"/>
       <c r="C115" s="24"/>
       <c r="D115" t="s">
         <v>297</v>
@@ -13617,7 +13672,7 @@
       <c r="A116" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="B116" s="40"/>
+      <c r="B116" s="38"/>
       <c r="C116" s="24"/>
       <c r="D116" t="s">
         <v>297</v>
@@ -13651,7 +13706,7 @@
       <c r="A117" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="B117" s="40"/>
+      <c r="B117" s="38"/>
       <c r="C117" s="24"/>
       <c r="D117" t="s">
         <v>297</v>
@@ -13685,7 +13740,7 @@
       <c r="A118" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="B118" s="40"/>
+      <c r="B118" s="38"/>
       <c r="C118" s="24"/>
       <c r="D118" t="s">
         <v>297</v>
@@ -13719,7 +13774,7 @@
       <c r="A119" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="B119" s="40"/>
+      <c r="B119" s="38"/>
       <c r="C119" s="24"/>
       <c r="D119" t="s">
         <v>297</v>
@@ -13753,7 +13808,7 @@
       <c r="A120" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="B120" s="40"/>
+      <c r="B120" s="38"/>
       <c r="C120" s="24"/>
       <c r="D120" t="s">
         <v>297</v>
@@ -13787,7 +13842,7 @@
       <c r="A121" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="B121" s="41"/>
+      <c r="B121" s="39"/>
       <c r="C121" s="31"/>
       <c r="D121" s="23" t="s">
         <v>297</v>
@@ -13855,11 +13910,11 @@
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B123" s="40"/>
-      <c r="C123" s="42"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="40"/>
       <c r="G123" s="18" t="s">
         <v>107</v>
       </c>
@@ -14090,9 +14145,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q129"/>
+  <autoFilter ref="A1:Q129" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>